<commit_message>
major improvements to the OCR algorithm
instead of checking whether the second word's centerY is within the first word's topY and bottomY, the algorithm now kind of iteratively works with a new approach. First, it sorts the words by y-coordinates. Then, it gets all words that are in the same line (by checking if the next word's topY is above all the other word's most bottomY with a margin of error of range Y / 3) and then sorts these words by x-coordinates. Finally, it adds this line of words to the ultimate string. Then, it proceeds with the next line and so on. Works like a charm with the previous 8 examples.
</commit_message>
<xml_diff>
--- a/solvia-vision/src/main/resources/excels/VergilerTest6i.xlsx
+++ b/solvia-vision/src/main/resources/excels/VergilerTest6i.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="31">
   <si>
     <t>Tarih</t>
   </si>
@@ -57,6 +57,54 @@
   </si>
   <si>
     <t>0</t>
+  </si>
+  <si>
+    <t>08/08/2022</t>
+  </si>
+  <si>
+    <t>GÜNEŞ GURME GIDA VE TUR.LTD.ŞTİ</t>
+  </si>
+  <si>
+    <t>0005</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4340766085 KOZYATAĞI </t>
+  </si>
+  <si>
+    <t>İST C8 APT.NO:21 ATAŞEHİR/ .</t>
+  </si>
+  <si>
+    <t>18.52</t>
+  </si>
+  <si>
+    <t>231.48</t>
+  </si>
+  <si>
+    <t>250.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4340766085 ZAMN KOZYATAĞI ZAMN </t>
+  </si>
+  <si>
+    <t>GIDA VE GÜNEŞ GURME TUR.LTD.ŞTİ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KOZYATAĞI </t>
+  </si>
+  <si>
+    <t>4340766085</t>
+  </si>
+  <si>
+    <t>GIDA VE BARBAROS SK GÜNEŞ GURME TUR.LTD.ŞTİ</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t xml:space="preserve">GÜNEŞ GURME GIDA VE TUR.LTD.ŞTİ </t>
+  </si>
+  <si>
+    <t xml:space="preserve">4340766085 </t>
   </si>
 </sst>
 </file>
@@ -101,7 +149,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="B2:I3"/>
+  <dimension ref="B2:I17"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -159,6 +207,370 @@
         <v>13</v>
       </c>
     </row>
+    <row r="4">
+      <c r="B4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G4" t="s">
+        <v>20</v>
+      </c>
+      <c r="H4" t="s">
+        <v>21</v>
+      </c>
+      <c r="I4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="B5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F5" t="s">
+        <v>19</v>
+      </c>
+      <c r="G5" t="s">
+        <v>20</v>
+      </c>
+      <c r="H5" t="s">
+        <v>21</v>
+      </c>
+      <c r="I5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="B6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6" t="s">
+        <v>23</v>
+      </c>
+      <c r="F6" t="s">
+        <v>19</v>
+      </c>
+      <c r="G6" t="s">
+        <v>20</v>
+      </c>
+      <c r="H6" t="s">
+        <v>21</v>
+      </c>
+      <c r="I6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="B7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7" t="s">
+        <v>17</v>
+      </c>
+      <c r="E7" t="s">
+        <v>23</v>
+      </c>
+      <c r="F7" t="s">
+        <v>19</v>
+      </c>
+      <c r="G7" t="s">
+        <v>20</v>
+      </c>
+      <c r="H7" t="s">
+        <v>21</v>
+      </c>
+      <c r="I7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="B8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" t="s">
+        <v>16</v>
+      </c>
+      <c r="D8" t="s">
+        <v>17</v>
+      </c>
+      <c r="E8" t="s">
+        <v>23</v>
+      </c>
+      <c r="F8" t="s">
+        <v>19</v>
+      </c>
+      <c r="G8" t="s">
+        <v>20</v>
+      </c>
+      <c r="H8" t="s">
+        <v>21</v>
+      </c>
+      <c r="I8" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="B9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" t="s">
+        <v>24</v>
+      </c>
+      <c r="D9" t="s">
+        <v>17</v>
+      </c>
+      <c r="E9" t="s">
+        <v>25</v>
+      </c>
+      <c r="F9" t="s">
+        <v>26</v>
+      </c>
+      <c r="G9" t="s">
+        <v>20</v>
+      </c>
+      <c r="H9" t="s">
+        <v>21</v>
+      </c>
+      <c r="I9" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="B10" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10" t="s">
+        <v>24</v>
+      </c>
+      <c r="D10" t="s">
+        <v>17</v>
+      </c>
+      <c r="E10" t="s">
+        <v>25</v>
+      </c>
+      <c r="F10" t="s">
+        <v>26</v>
+      </c>
+      <c r="G10" t="s">
+        <v>20</v>
+      </c>
+      <c r="H10" t="s">
+        <v>21</v>
+      </c>
+      <c r="I10" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="B11" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" t="s">
+        <v>24</v>
+      </c>
+      <c r="D11" t="s">
+        <v>17</v>
+      </c>
+      <c r="E11" t="s">
+        <v>25</v>
+      </c>
+      <c r="F11" t="s">
+        <v>26</v>
+      </c>
+      <c r="G11" t="s">
+        <v>20</v>
+      </c>
+      <c r="H11" t="s">
+        <v>21</v>
+      </c>
+      <c r="I11" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="B12" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12" t="s">
+        <v>24</v>
+      </c>
+      <c r="D12" t="s">
+        <v>17</v>
+      </c>
+      <c r="E12" t="s">
+        <v>25</v>
+      </c>
+      <c r="F12" t="s">
+        <v>26</v>
+      </c>
+      <c r="G12" t="s">
+        <v>20</v>
+      </c>
+      <c r="H12" t="s">
+        <v>21</v>
+      </c>
+      <c r="I12" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="B13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C13" t="s">
+        <v>24</v>
+      </c>
+      <c r="D13" t="s">
+        <v>17</v>
+      </c>
+      <c r="E13" t="s">
+        <v>25</v>
+      </c>
+      <c r="F13" t="s">
+        <v>26</v>
+      </c>
+      <c r="G13" t="s">
+        <v>20</v>
+      </c>
+      <c r="H13" t="s">
+        <v>21</v>
+      </c>
+      <c r="I13" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="B14" t="s">
+        <v>15</v>
+      </c>
+      <c r="C14" t="s">
+        <v>27</v>
+      </c>
+      <c r="D14" t="s">
+        <v>28</v>
+      </c>
+      <c r="E14" t="s">
+        <v>25</v>
+      </c>
+      <c r="F14" t="s">
+        <v>26</v>
+      </c>
+      <c r="G14" t="s">
+        <v>20</v>
+      </c>
+      <c r="H14" t="s">
+        <v>21</v>
+      </c>
+      <c r="I14" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="B15" t="s">
+        <v>15</v>
+      </c>
+      <c r="C15" t="s">
+        <v>24</v>
+      </c>
+      <c r="D15" t="s">
+        <v>17</v>
+      </c>
+      <c r="E15" t="s">
+        <v>25</v>
+      </c>
+      <c r="F15" t="s">
+        <v>26</v>
+      </c>
+      <c r="G15" t="s">
+        <v>20</v>
+      </c>
+      <c r="H15" t="s">
+        <v>21</v>
+      </c>
+      <c r="I15" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="B16" t="s">
+        <v>15</v>
+      </c>
+      <c r="C16" t="s">
+        <v>24</v>
+      </c>
+      <c r="D16" t="s">
+        <v>17</v>
+      </c>
+      <c r="E16" t="s">
+        <v>25</v>
+      </c>
+      <c r="F16" t="s">
+        <v>26</v>
+      </c>
+      <c r="G16" t="s">
+        <v>20</v>
+      </c>
+      <c r="H16" t="s">
+        <v>21</v>
+      </c>
+      <c r="I16" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="B17" t="s">
+        <v>15</v>
+      </c>
+      <c r="C17" t="s">
+        <v>29</v>
+      </c>
+      <c r="D17" t="s">
+        <v>17</v>
+      </c>
+      <c r="E17" t="s">
+        <v>25</v>
+      </c>
+      <c r="F17" t="s">
+        <v>30</v>
+      </c>
+      <c r="G17" t="s">
+        <v>20</v>
+      </c>
+      <c r="H17" t="s">
+        <v>21</v>
+      </c>
+      <c r="I17" t="s">
+        <v>22</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>